<commit_message>
1. updated world map data from overall to overage 2. added Jaimaica data 3. updated code formatting and comment
</commit_message>
<xml_diff>
--- a/raw_data/social_immigrants/employment_by_country.xlsx
+++ b/raw_data/social_immigrants/employment_by_country.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mengxit/Dropbox/MDE/Fall 2019/Data Gov1005/Projects/final_project/US-Immigration-Explorer/raw_data/english_speaking_immigrants/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mengxi/Dropbox/MDE/Fall 2019/Data Gov1005/Projects/final_project/US-Immigration-Explorer/raw_data/social_immigrants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{890DD7AA-4ADD-934F-A68B-CF478ED5B2C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA9722A-43F5-A642-A0EA-A1B0E5294EDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16120" xr2:uid="{B4FC126C-EE5C-274C-B23B-89AB2DE5F349}"/>
+    <workbookView xWindow="11540" yWindow="7160" windowWidth="27640" windowHeight="16120" xr2:uid="{B4FC126C-EE5C-274C-B23B-89AB2DE5F349}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="20">
   <si>
     <t>Colombia</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Total Number</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
   </si>
 </sst>
 </file>
@@ -487,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD7C6D8C-80FF-0345-89A4-B6126F108D87}">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,22 +545,22 @@
         <v>0.42199999999999999</v>
       </c>
       <c r="C2" s="3">
-        <f>1-B2</f>
+        <f t="shared" ref="C2:C33" si="0">1-B2</f>
         <v>0.57800000000000007</v>
       </c>
       <c r="D2">
-        <f>A2*C2</f>
+        <f t="shared" ref="D2:D33" si="1">A2*C2</f>
         <v>1206327.0380000002</v>
       </c>
       <c r="E2" s="1">
         <v>2.4E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2/C2</f>
+        <f t="shared" ref="F2:F33" si="2">E2/C2</f>
         <v>4.1522491349480967E-2</v>
       </c>
       <c r="G2">
-        <f>A2*E2</f>
+        <f t="shared" ref="G2:G33" si="3">A2*E2</f>
         <v>50089.703999999998</v>
       </c>
       <c r="H2">
@@ -575,22 +578,22 @@
         <v>0.432</v>
       </c>
       <c r="C3" s="3">
-        <f>1-B3</f>
+        <f t="shared" si="0"/>
         <v>0.56800000000000006</v>
       </c>
       <c r="D3">
-        <f>A3*C3</f>
+        <f t="shared" si="1"/>
         <v>1135846.0720000002</v>
       </c>
       <c r="E3" s="1">
         <v>2.4E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3/C3</f>
+        <f t="shared" si="2"/>
         <v>4.2253521126760563E-2</v>
       </c>
       <c r="G3">
-        <f>A3*E3</f>
+        <f t="shared" si="3"/>
         <v>47993.495999999999</v>
       </c>
       <c r="H3">
@@ -608,22 +611,22 @@
         <v>0.42899999999999999</v>
       </c>
       <c r="C4" s="3">
-        <f>1-B4</f>
+        <f t="shared" si="0"/>
         <v>0.57099999999999995</v>
       </c>
       <c r="D4">
-        <f>A4*C4</f>
+        <f t="shared" si="1"/>
         <v>1107996.95</v>
       </c>
       <c r="E4" s="1">
         <v>0.03</v>
       </c>
       <c r="F4" s="1">
-        <f>E4/C4</f>
+        <f t="shared" si="2"/>
         <v>5.2539404553415062E-2</v>
       </c>
       <c r="G4">
-        <f>A4*E4</f>
+        <f t="shared" si="3"/>
         <v>58213.5</v>
       </c>
       <c r="H4">
@@ -641,22 +644,22 @@
         <v>0.43</v>
       </c>
       <c r="C5" s="3">
-        <f>1-B5</f>
+        <f t="shared" si="0"/>
         <v>0.57000000000000006</v>
       </c>
       <c r="D5">
-        <f>A5*C5</f>
+        <f t="shared" si="1"/>
         <v>1029521.4600000001</v>
       </c>
       <c r="E5" s="1">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5/C5</f>
+        <f t="shared" si="2"/>
         <v>5.6140350877192977E-2</v>
       </c>
       <c r="G5">
-        <f>A5*E5</f>
+        <f t="shared" si="3"/>
         <v>57797.696000000004</v>
       </c>
       <c r="H5">
@@ -674,22 +677,22 @@
         <v>0.42399999999999999</v>
       </c>
       <c r="C6" s="3">
-        <f>1-B6</f>
+        <f t="shared" si="0"/>
         <v>0.57600000000000007</v>
       </c>
       <c r="D6">
-        <f>A6*C6</f>
+        <f t="shared" si="1"/>
         <v>971525.37600000016</v>
       </c>
       <c r="E6" s="1">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6/C6</f>
+        <f t="shared" si="2"/>
         <v>6.597222222222221E-2</v>
       </c>
       <c r="G6">
-        <f>A6*E6</f>
+        <f t="shared" si="3"/>
         <v>64093.688000000002</v>
       </c>
       <c r="H6">
@@ -707,22 +710,22 @@
         <v>0.41199999999999998</v>
       </c>
       <c r="C7" s="3">
-        <f>1-B7</f>
+        <f t="shared" si="0"/>
         <v>0.58800000000000008</v>
       </c>
       <c r="D7">
-        <f>A7*C7</f>
+        <f t="shared" si="1"/>
         <v>937929.97200000007</v>
       </c>
       <c r="E7" s="1">
         <v>0.04</v>
       </c>
       <c r="F7" s="1">
-        <f>E7/C7</f>
+        <f t="shared" si="2"/>
         <v>6.8027210884353734E-2</v>
       </c>
       <c r="G7">
-        <f>A7*E7</f>
+        <f t="shared" si="3"/>
         <v>63804.76</v>
       </c>
       <c r="H7">
@@ -740,22 +743,22 @@
         <v>0.4</v>
       </c>
       <c r="C8" s="3">
-        <f>1-B8</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="D8">
-        <f>A8*C8</f>
+        <f t="shared" si="1"/>
         <v>919465.79999999993</v>
       </c>
       <c r="E8" s="1">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8/C8</f>
+        <f t="shared" si="2"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G8">
-        <f>A8*E8</f>
+        <f t="shared" si="3"/>
         <v>64362.606000000007</v>
       </c>
       <c r="H8">
@@ -773,22 +776,22 @@
         <v>0.38500000000000001</v>
       </c>
       <c r="C9" s="3">
-        <f>1-B9</f>
+        <f t="shared" si="0"/>
         <v>0.61499999999999999</v>
       </c>
       <c r="D9">
-        <f>A9*C9</f>
+        <f t="shared" si="1"/>
         <v>912568.98</v>
       </c>
       <c r="E9" s="1">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9/C9</f>
+        <f t="shared" si="2"/>
         <v>8.2926829268292673E-2</v>
       </c>
       <c r="G9">
-        <f>A9*E9</f>
+        <f t="shared" si="3"/>
         <v>75676.45199999999</v>
       </c>
       <c r="H9">
@@ -806,22 +809,22 @@
         <v>0.374</v>
       </c>
       <c r="C10" s="3">
-        <f>1-B10</f>
+        <f t="shared" si="0"/>
         <v>0.626</v>
       </c>
       <c r="D10">
-        <f>A10*C10</f>
+        <f t="shared" si="1"/>
         <v>826566.01800000004</v>
       </c>
       <c r="E10" s="1">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10/C10</f>
+        <f t="shared" si="2"/>
         <v>7.8274760383386585E-2</v>
       </c>
       <c r="G10">
-        <f>A10*E10</f>
+        <f t="shared" si="3"/>
         <v>64699.257000000005</v>
       </c>
       <c r="H10">
@@ -839,22 +842,22 @@
         <v>0.375</v>
       </c>
       <c r="C11" s="3">
-        <f>1-B11</f>
+        <f t="shared" si="0"/>
         <v>0.625</v>
       </c>
       <c r="D11">
-        <f>A11*C11</f>
+        <f t="shared" si="1"/>
         <v>787380.625</v>
       </c>
       <c r="E11" s="1">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11/C11</f>
+        <f t="shared" si="2"/>
         <v>5.1200000000000002E-2</v>
       </c>
       <c r="G11">
-        <f>A11*E11</f>
+        <f t="shared" si="3"/>
         <v>40313.887999999999</v>
       </c>
       <c r="H11">
@@ -872,22 +875,22 @@
         <v>0.38400000000000001</v>
       </c>
       <c r="C12" s="8">
-        <f>1-B12</f>
+        <f t="shared" si="0"/>
         <v>0.61599999999999999</v>
       </c>
       <c r="D12" s="6">
-        <f>A12*C12</f>
+        <f t="shared" si="1"/>
         <v>776098.4</v>
       </c>
       <c r="E12" s="10">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F12" s="7">
-        <f>E12/C12</f>
+        <f t="shared" si="2"/>
         <v>4.2207792207792208E-2</v>
       </c>
       <c r="G12" s="6">
-        <f>A12*E12</f>
+        <f t="shared" si="3"/>
         <v>32757.399999999998</v>
       </c>
       <c r="H12" s="6">
@@ -905,22 +908,22 @@
         <v>0.314</v>
       </c>
       <c r="C13" s="3">
-        <f>1-B13</f>
+        <f t="shared" si="0"/>
         <v>0.68599999999999994</v>
       </c>
       <c r="D13">
-        <f>A13*C13</f>
+        <f t="shared" si="1"/>
         <v>7496320.5659999996</v>
       </c>
       <c r="E13" s="1">
         <v>0.03</v>
       </c>
       <c r="F13" s="1">
-        <f>E13/C13</f>
+        <f t="shared" si="2"/>
         <v>4.3731778425655982E-2</v>
       </c>
       <c r="G13">
-        <f>A13*E13</f>
+        <f t="shared" si="3"/>
         <v>327827.43</v>
       </c>
       <c r="H13">
@@ -938,22 +941,22 @@
         <v>0.311</v>
       </c>
       <c r="C14" s="3">
-        <f>1-B14</f>
+        <f t="shared" si="0"/>
         <v>0.68900000000000006</v>
       </c>
       <c r="D14">
-        <f>A14*C14</f>
+        <f t="shared" si="1"/>
         <v>7720577.0980000002</v>
       </c>
       <c r="E14" s="1">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14/C14</f>
+        <f t="shared" si="2"/>
         <v>4.9346879535558781E-2</v>
       </c>
       <c r="G14">
-        <f>A14*E14</f>
+        <f t="shared" si="3"/>
         <v>380986.38800000004</v>
       </c>
       <c r="H14">
@@ -971,22 +974,22 @@
         <v>0.312</v>
       </c>
       <c r="C15" s="3">
-        <f>1-B15</f>
+        <f t="shared" si="0"/>
         <v>0.68799999999999994</v>
       </c>
       <c r="D15">
-        <f>A15*C15</f>
+        <f t="shared" si="1"/>
         <v>7731953.8399999989</v>
       </c>
       <c r="E15" s="1">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15/C15</f>
+        <f t="shared" si="2"/>
         <v>5.3779069767441859E-2</v>
       </c>
       <c r="G15">
-        <f>A15*E15</f>
+        <f t="shared" si="3"/>
         <v>415817.28499999997</v>
       </c>
       <c r="H15">
@@ -1004,22 +1007,22 @@
         <v>0.311</v>
       </c>
       <c r="C16" s="3">
-        <f>1-B16</f>
+        <f t="shared" si="0"/>
         <v>0.68900000000000006</v>
       </c>
       <c r="D16">
-        <f>A16*C16</f>
+        <f t="shared" si="1"/>
         <v>7755084.9740000004</v>
       </c>
       <c r="E16" s="1">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16/C16</f>
+        <f t="shared" si="2"/>
         <v>6.3860667634252535E-2</v>
       </c>
       <c r="G16">
-        <f>A16*E16</f>
+        <f t="shared" si="3"/>
         <v>495244.90399999998</v>
       </c>
       <c r="H16">
@@ -1037,22 +1040,22 @@
         <v>0.30499999999999999</v>
       </c>
       <c r="C17" s="3">
-        <f>1-B17</f>
+        <f t="shared" si="0"/>
         <v>0.69500000000000006</v>
       </c>
       <c r="D17">
-        <f>A17*C17</f>
+        <f t="shared" si="1"/>
         <v>7689664.870000001</v>
       </c>
       <c r="E17" s="2">
         <v>5.5E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17/C17</f>
+        <f t="shared" si="2"/>
         <v>7.9136690647482008E-2</v>
       </c>
       <c r="G17">
-        <f>A17*E17</f>
+        <f t="shared" si="3"/>
         <v>608534.63</v>
       </c>
       <c r="H17">
@@ -1070,22 +1073,22 @@
         <v>0.309</v>
       </c>
       <c r="C18" s="3">
-        <f>1-B18</f>
+        <f t="shared" si="0"/>
         <v>0.69100000000000006</v>
       </c>
       <c r="D18">
-        <f>A18*C18</f>
+        <f t="shared" si="1"/>
         <v>7598564.2250000006</v>
       </c>
       <c r="E18" s="1">
         <v>6.3E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18/C18</f>
+        <f t="shared" si="2"/>
         <v>9.1172214182344419E-2</v>
       </c>
       <c r="G18">
-        <f>A18*E18</f>
+        <f t="shared" si="3"/>
         <v>692777.92500000005</v>
       </c>
       <c r="H18">
@@ -1103,22 +1106,22 @@
         <v>0.30599999999999999</v>
       </c>
       <c r="C19" s="3">
-        <f>1-B19</f>
+        <f t="shared" si="0"/>
         <v>0.69399999999999995</v>
       </c>
       <c r="D19">
-        <f>A19*C19</f>
+        <f t="shared" si="1"/>
         <v>7658502.3639999991</v>
       </c>
       <c r="E19" s="1">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19/C19</f>
+        <f t="shared" si="2"/>
         <v>0.10230547550432277</v>
       </c>
       <c r="G19">
-        <f>A19*E19</f>
+        <f t="shared" si="3"/>
         <v>783506.72599999991</v>
       </c>
       <c r="H19">
@@ -1136,22 +1139,22 @@
         <v>0.3</v>
       </c>
       <c r="C20" s="3">
-        <f>1-B20</f>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
       <c r="D20">
-        <f>A20*C20</f>
+        <f t="shared" si="1"/>
         <v>7695443.6999999993</v>
       </c>
       <c r="E20" s="1">
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="F20" s="1">
-        <f>E20/C20</f>
+        <f t="shared" si="2"/>
         <v>0.11</v>
       </c>
       <c r="G20">
-        <f>A20*E20</f>
+        <f t="shared" si="3"/>
         <v>846498.80700000003</v>
       </c>
       <c r="H20">
@@ -1169,22 +1172,22 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="C21" s="3">
-        <f>1-B21</f>
+        <f t="shared" si="0"/>
         <v>0.71399999999999997</v>
       </c>
       <c r="D21">
-        <f>A21*C21</f>
+        <f t="shared" si="1"/>
         <v>7655984.2379999999</v>
       </c>
       <c r="E21" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>E21/C21</f>
+        <f t="shared" si="2"/>
         <v>0.10504201680672269</v>
       </c>
       <c r="G21">
-        <f>A21*E21</f>
+        <f t="shared" si="3"/>
         <v>804200.02500000002</v>
       </c>
       <c r="H21">
@@ -1202,22 +1205,22 @@
         <v>0.28399999999999997</v>
       </c>
       <c r="C22" s="3">
-        <f>1-B22</f>
+        <f t="shared" si="0"/>
         <v>0.71599999999999997</v>
       </c>
       <c r="D22">
-        <f>A22*C22</f>
+        <f t="shared" si="1"/>
         <v>7592675.9359999998</v>
       </c>
       <c r="E22" s="1">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F22" s="1">
-        <f>E22/C22</f>
+        <f t="shared" si="2"/>
         <v>6.2849162011173187E-2</v>
       </c>
       <c r="G22">
-        <f>A22*E22</f>
+        <f t="shared" si="3"/>
         <v>477193.32</v>
       </c>
       <c r="H22">
@@ -1235,22 +1238,22 @@
         <v>0.29899999999999999</v>
       </c>
       <c r="C23" s="8">
-        <f>1-B23</f>
+        <f t="shared" si="0"/>
         <v>0.70100000000000007</v>
       </c>
       <c r="D23" s="6">
-        <f>A23*C23</f>
+        <f t="shared" si="1"/>
         <v>7609229.5210000006</v>
       </c>
       <c r="E23" s="7">
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="F23" s="7">
-        <f>E23/C23</f>
+        <f t="shared" si="2"/>
         <v>5.8487874465049924E-2</v>
       </c>
       <c r="G23" s="6">
-        <f>A23*E23</f>
+        <f t="shared" si="3"/>
         <v>445047.66100000002</v>
       </c>
       <c r="H23" s="6">
@@ -1268,22 +1271,22 @@
         <v>0.29899999999999999</v>
       </c>
       <c r="C24" s="3">
-        <f>1-B24</f>
+        <f t="shared" si="0"/>
         <v>0.70100000000000007</v>
       </c>
       <c r="D24">
-        <f>A24*C24</f>
+        <f t="shared" si="1"/>
         <v>1717513.09</v>
       </c>
       <c r="E24" s="1">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="F24" s="1">
-        <f>E24/C24</f>
+        <f t="shared" si="2"/>
         <v>3.566333808844508E-2</v>
       </c>
       <c r="G24">
-        <f>A24*E24</f>
+        <f t="shared" si="3"/>
         <v>61252.25</v>
       </c>
       <c r="H24">
@@ -1301,22 +1304,22 @@
         <v>0.30299999999999999</v>
       </c>
       <c r="C25" s="3">
-        <f>1-B25</f>
+        <f t="shared" si="0"/>
         <v>0.69700000000000006</v>
       </c>
       <c r="D25">
-        <f>A25*C25</f>
+        <f t="shared" si="1"/>
         <v>1592474.932</v>
       </c>
       <c r="E25" s="1">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="F25" s="1">
-        <f>E25/C25</f>
+        <f t="shared" si="2"/>
         <v>4.0172166427546625E-2</v>
       </c>
       <c r="G25">
-        <f>A25*E25</f>
+        <f t="shared" si="3"/>
         <v>63973.167999999998</v>
       </c>
       <c r="H25">
@@ -1334,22 +1337,22 @@
         <v>0.30299999999999999</v>
       </c>
       <c r="C26" s="3">
-        <f>1-B26</f>
+        <f t="shared" si="0"/>
         <v>0.69700000000000006</v>
       </c>
       <c r="D26">
-        <f>A26*C26</f>
+        <f t="shared" si="1"/>
         <v>1592474.932</v>
       </c>
       <c r="E26" s="1">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="F26" s="1">
-        <f>E26/C26</f>
+        <f t="shared" si="2"/>
         <v>4.0172166427546625E-2</v>
       </c>
       <c r="G26">
-        <f>A26*E26</f>
+        <f t="shared" si="3"/>
         <v>63973.167999999998</v>
       </c>
       <c r="H26">
@@ -1367,22 +1370,22 @@
         <v>0.307</v>
       </c>
       <c r="C27" s="3">
-        <f>1-B27</f>
+        <f t="shared" si="0"/>
         <v>0.69300000000000006</v>
       </c>
       <c r="D27">
-        <f>A27*C27</f>
+        <f t="shared" si="1"/>
         <v>1441873.1250000002</v>
       </c>
       <c r="E27" s="1">
         <v>3.1E-2</v>
       </c>
       <c r="F27" s="1">
-        <f>E27/C27</f>
+        <f t="shared" si="2"/>
         <v>4.4733044733044729E-2</v>
       </c>
       <c r="G27">
-        <f>A27*E27</f>
+        <f t="shared" si="3"/>
         <v>64499.375</v>
       </c>
       <c r="H27">
@@ -1400,22 +1403,22 @@
         <v>0.30099999999999999</v>
       </c>
       <c r="C28" s="3">
-        <f>1-B28</f>
+        <f t="shared" si="0"/>
         <v>0.69900000000000007</v>
       </c>
       <c r="D28">
-        <f>A28*C28</f>
+        <f t="shared" si="1"/>
         <v>1349299.2720000001</v>
       </c>
       <c r="E28" s="1">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="F28" s="1">
-        <f>E28/C28</f>
+        <f t="shared" si="2"/>
         <v>5.1502145922746774E-2</v>
       </c>
       <c r="G28">
-        <f>A28*E28</f>
+        <f t="shared" si="3"/>
         <v>69491.80799999999</v>
       </c>
       <c r="H28">
@@ -1433,22 +1436,22 @@
         <v>0.28699999999999998</v>
       </c>
       <c r="C29" s="3">
-        <f>1-B29</f>
+        <f t="shared" si="0"/>
         <v>0.71300000000000008</v>
       </c>
       <c r="D29">
-        <f>A29*C29</f>
+        <f t="shared" si="1"/>
         <v>1331905.3900000001</v>
       </c>
       <c r="E29" s="1">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="F29" s="1">
-        <f>E29/C29</f>
+        <f t="shared" si="2"/>
         <v>5.3295932678821871E-2</v>
       </c>
       <c r="G29">
-        <f>A29*E29</f>
+        <f t="shared" si="3"/>
         <v>70985.14</v>
       </c>
       <c r="H29">
@@ -1466,22 +1469,22 @@
         <v>0.29099999999999998</v>
       </c>
       <c r="C30" s="3">
-        <f>1-B30</f>
+        <f t="shared" si="0"/>
         <v>0.70900000000000007</v>
       </c>
       <c r="D30">
-        <f>A30*C30</f>
+        <f t="shared" si="1"/>
         <v>1247913.0270000002</v>
       </c>
       <c r="E30" s="1">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="F30" s="1">
-        <f>E30/C30</f>
+        <f t="shared" si="2"/>
         <v>6.0648801128349777E-2</v>
       </c>
       <c r="G30">
-        <f>A30*E30</f>
+        <f t="shared" si="3"/>
         <v>75684.428999999989</v>
       </c>
       <c r="H30">
@@ -1499,22 +1502,22 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="C31" s="3">
-        <f>1-B31</f>
+        <f t="shared" si="0"/>
         <v>0.71399999999999997</v>
       </c>
       <c r="D31">
-        <f>A31*C31</f>
+        <f t="shared" si="1"/>
         <v>1204050.3299999998</v>
       </c>
       <c r="E31" s="1">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="F31" s="1">
-        <f>E31/C31</f>
+        <f t="shared" si="2"/>
         <v>6.8627450980392163E-2</v>
       </c>
       <c r="G31">
-        <f>A31*E31</f>
+        <f t="shared" si="3"/>
         <v>82630.904999999999</v>
       </c>
       <c r="H31">
@@ -1532,22 +1535,22 @@
         <v>0.27900000000000003</v>
       </c>
       <c r="C32" s="3">
-        <f>1-B32</f>
+        <f t="shared" si="0"/>
         <v>0.72099999999999997</v>
       </c>
       <c r="D32">
-        <f>A32*C32</f>
+        <f t="shared" si="1"/>
         <v>1134075.32</v>
       </c>
       <c r="E32" s="1">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F32" s="1">
-        <f>E32/C32</f>
+        <f t="shared" si="2"/>
         <v>6.6574202496532592E-2</v>
       </c>
       <c r="G32">
-        <f>A32*E32</f>
+        <f t="shared" si="3"/>
         <v>75500.160000000003</v>
       </c>
       <c r="H32">
@@ -1565,22 +1568,22 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="C33" s="3">
-        <f>1-B33</f>
+        <f t="shared" si="0"/>
         <v>0.72</v>
       </c>
       <c r="D33">
-        <f>A33*C33</f>
+        <f t="shared" si="1"/>
         <v>1099494</v>
       </c>
       <c r="E33" s="1">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="F33" s="1">
-        <f>E33/C33</f>
+        <f t="shared" si="2"/>
         <v>4.4444444444444446E-2</v>
       </c>
       <c r="G33">
-        <f>A33*E33</f>
+        <f t="shared" si="3"/>
         <v>48866.400000000001</v>
       </c>
       <c r="H33">
@@ -1598,22 +1601,22 @@
         <v>0.29899999999999999</v>
       </c>
       <c r="C34" s="8">
-        <f>1-B34</f>
+        <f t="shared" ref="C34:C65" si="4">1-B34</f>
         <v>0.70100000000000007</v>
       </c>
       <c r="D34" s="6">
-        <f>A34*C34</f>
+        <f t="shared" ref="D34:D65" si="5">A34*C34</f>
         <v>997678.62200000009</v>
       </c>
       <c r="E34" s="7">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="F34" s="7">
-        <f>E34/C34</f>
+        <f t="shared" ref="F34:F65" si="6">E34/C34</f>
         <v>4.136947218259629E-2</v>
       </c>
       <c r="G34" s="6">
-        <f>A34*E34</f>
+        <f t="shared" ref="G34:G65" si="7">A34*E34</f>
         <v>41273.438000000002</v>
       </c>
       <c r="H34" s="6">
@@ -1631,22 +1634,22 @@
         <v>0.36499999999999999</v>
       </c>
       <c r="C35" s="3">
-        <f>1-B35</f>
+        <f t="shared" si="4"/>
         <v>0.63500000000000001</v>
       </c>
       <c r="D35">
-        <f>A35*C35</f>
+        <f t="shared" si="5"/>
         <v>415174.43</v>
       </c>
       <c r="E35" s="1">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F35" s="1">
-        <f>E35/C35</f>
+        <f t="shared" si="6"/>
         <v>4.0944881889763779E-2</v>
       </c>
       <c r="G35">
-        <f>A35*E35</f>
+        <f t="shared" si="7"/>
         <v>16999.268</v>
       </c>
       <c r="H35">
@@ -1664,22 +1667,22 @@
         <v>0.374</v>
       </c>
       <c r="C36" s="3">
-        <f>1-B36</f>
+        <f t="shared" si="4"/>
         <v>0.626</v>
       </c>
       <c r="D36">
-        <f>A36*C36</f>
+        <f t="shared" si="5"/>
         <v>363371.09</v>
       </c>
       <c r="E36" s="1">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="F36" s="1">
-        <f>E36/C36</f>
+        <f t="shared" si="6"/>
         <v>7.3482428115015971E-2</v>
       </c>
       <c r="G36">
-        <f>A36*E36</f>
+        <f t="shared" si="7"/>
         <v>26701.39</v>
       </c>
       <c r="H36">
@@ -1697,22 +1700,22 @@
         <v>0.373</v>
       </c>
       <c r="C37" s="3">
-        <f>1-B37</f>
+        <f t="shared" si="4"/>
         <v>0.627</v>
       </c>
       <c r="D37">
-        <f>A37*C37</f>
+        <f t="shared" si="5"/>
         <v>380683.05</v>
       </c>
       <c r="E37" s="1">
         <v>2.7E-2</v>
       </c>
       <c r="F37" s="1">
-        <f>E37/C37</f>
+        <f t="shared" si="6"/>
         <v>4.3062200956937802E-2</v>
       </c>
       <c r="G37">
-        <f>A37*E37</f>
+        <f t="shared" si="7"/>
         <v>16393.05</v>
       </c>
       <c r="H37">
@@ -1730,22 +1733,22 @@
         <v>0.38500000000000001</v>
       </c>
       <c r="C38" s="3">
-        <f>1-B38</f>
+        <f t="shared" si="4"/>
         <v>0.61499999999999999</v>
       </c>
       <c r="D38">
-        <f>A38*C38</f>
+        <f t="shared" si="5"/>
         <v>362683.33500000002</v>
       </c>
       <c r="E38" s="1">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="F38" s="1">
-        <f>E38/C38</f>
+        <f t="shared" si="6"/>
         <v>5.2032520325203252E-2</v>
       </c>
       <c r="G38">
-        <f>A38*E38</f>
+        <f t="shared" si="7"/>
         <v>18871.328000000001</v>
       </c>
       <c r="H38">
@@ -1763,22 +1766,22 @@
         <v>0.38</v>
       </c>
       <c r="C39" s="3">
-        <f>1-B39</f>
+        <f t="shared" si="4"/>
         <v>0.62</v>
       </c>
       <c r="D39">
-        <f>A39*C39</f>
+        <f t="shared" si="5"/>
         <v>351373.22</v>
       </c>
       <c r="E39" s="1">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="F39" s="1">
-        <f>E39/C39</f>
+        <f t="shared" si="6"/>
         <v>5.4838709677419356E-2</v>
       </c>
       <c r="G39">
-        <f>A39*E39</f>
+        <f t="shared" si="7"/>
         <v>19268.854000000003</v>
       </c>
       <c r="H39">
@@ -1796,22 +1799,22 @@
         <v>0.40300000000000002</v>
       </c>
       <c r="C40" s="3">
-        <f>1-B40</f>
+        <f t="shared" si="4"/>
         <v>0.59699999999999998</v>
       </c>
       <c r="D40">
-        <f>A40*C40</f>
+        <f t="shared" si="5"/>
         <v>344689.29300000001</v>
       </c>
       <c r="E40" s="1">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="F40" s="1">
-        <f>E40/C40</f>
+        <f t="shared" si="6"/>
         <v>6.030150753768844E-2</v>
       </c>
       <c r="G40">
-        <f>A40*E40</f>
+        <f t="shared" si="7"/>
         <v>20785.284</v>
       </c>
       <c r="H40">
@@ -1829,22 +1832,22 @@
         <v>0.4</v>
       </c>
       <c r="C41" s="3">
-        <f>1-B41</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="D41">
-        <f>A41*C41</f>
+        <f t="shared" si="5"/>
         <v>350272.2</v>
       </c>
       <c r="E41" s="1">
         <v>0.04</v>
       </c>
       <c r="F41" s="1">
-        <f>E41/C41</f>
+        <f t="shared" si="6"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="G41">
-        <f>A41*E41</f>
+        <f t="shared" si="7"/>
         <v>23351.48</v>
       </c>
       <c r="H41">
@@ -1862,22 +1865,22 @@
         <v>0.371</v>
       </c>
       <c r="C42" s="3">
-        <f>1-B42</f>
+        <f t="shared" si="4"/>
         <v>0.629</v>
       </c>
       <c r="D42">
-        <f>A42*C42</f>
+        <f t="shared" si="5"/>
         <v>364082.18300000002</v>
       </c>
       <c r="E42" s="1">
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="F42" s="1">
-        <f>E42/C42</f>
+        <f t="shared" si="6"/>
         <v>8.2670906200317959E-2</v>
       </c>
       <c r="G42">
-        <f>A42*E42</f>
+        <f t="shared" si="7"/>
         <v>30099.003999999997</v>
       </c>
       <c r="H42">
@@ -1895,22 +1898,22 @@
         <v>0.379</v>
       </c>
       <c r="C43" s="3">
-        <f>1-B43</f>
+        <f t="shared" si="4"/>
         <v>0.621</v>
       </c>
       <c r="D43">
-        <f>A43*C43</f>
+        <f t="shared" si="5"/>
         <v>305055.07199999999</v>
       </c>
       <c r="E43" s="1">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="F43" s="1">
-        <f>E43/C43</f>
+        <f t="shared" si="6"/>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="G43">
-        <f>A43*E43</f>
+        <f t="shared" si="7"/>
         <v>22596.671999999999</v>
       </c>
       <c r="H43">
@@ -1928,22 +1931,22 @@
         <v>0.35799999999999998</v>
       </c>
       <c r="C44" s="3">
-        <f>1-B44</f>
+        <f t="shared" si="4"/>
         <v>0.64200000000000002</v>
       </c>
       <c r="D44">
-        <f>A44*C44</f>
+        <f t="shared" si="5"/>
         <v>299921.21399999998</v>
       </c>
       <c r="E44" s="1">
         <v>3.1E-2</v>
       </c>
       <c r="F44" s="1">
-        <f>E44/C44</f>
+        <f t="shared" si="6"/>
         <v>4.8286604361370715E-2</v>
       </c>
       <c r="G44">
-        <f>A44*E44</f>
+        <f t="shared" si="7"/>
         <v>14482.177</v>
       </c>
       <c r="H44">
@@ -1961,22 +1964,22 @@
         <v>0.4</v>
       </c>
       <c r="C45" s="8">
-        <f>1-B45</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="D45" s="6">
-        <f>A45*C45</f>
+        <f t="shared" si="5"/>
         <v>292016.39999999997</v>
       </c>
       <c r="E45" s="7">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F45" s="7">
-        <f>E45/C45</f>
+        <f t="shared" si="6"/>
         <v>4.3333333333333335E-2</v>
       </c>
       <c r="G45" s="6">
-        <f>A45*E45</f>
+        <f t="shared" si="7"/>
         <v>12654.044</v>
       </c>
       <c r="H45" s="6">
@@ -1994,22 +1997,22 @@
         <v>0.32600000000000001</v>
       </c>
       <c r="C46" s="3">
-        <f>1-B46</f>
+        <f t="shared" si="4"/>
         <v>0.67399999999999993</v>
       </c>
       <c r="D46">
-        <f>A46*C46</f>
+        <f t="shared" si="5"/>
         <v>1308479.3359999999</v>
       </c>
       <c r="E46" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F46" s="1">
-        <f>E46/C46</f>
+        <f t="shared" si="6"/>
         <v>3.2640949554896145E-2</v>
       </c>
       <c r="G46">
-        <f>A46*E46</f>
+        <f t="shared" si="7"/>
         <v>42710.007999999994</v>
       </c>
       <c r="H46">
@@ -2027,22 +2030,22 @@
         <v>0.33100000000000002</v>
       </c>
       <c r="C47" s="3">
-        <f>1-B47</f>
+        <f t="shared" si="4"/>
         <v>0.66900000000000004</v>
       </c>
       <c r="D47">
-        <f>A47*C47</f>
+        <f t="shared" si="5"/>
         <v>1258193.652</v>
       </c>
       <c r="E47" s="1">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F47" s="1">
-        <f>E47/C47</f>
+        <f t="shared" si="6"/>
         <v>3.8863976083707022E-2</v>
       </c>
       <c r="G47">
-        <f>A47*E47</f>
+        <f t="shared" si="7"/>
         <v>48898.407999999996</v>
       </c>
       <c r="H47">
@@ -2060,22 +2063,22 @@
         <v>0.32100000000000001</v>
       </c>
       <c r="C48" s="3">
-        <f>1-B48</f>
+        <f t="shared" si="4"/>
         <v>0.67900000000000005</v>
       </c>
       <c r="D48">
-        <f>A48*C48</f>
+        <f t="shared" si="5"/>
         <v>1293005.4410000001</v>
       </c>
       <c r="E48" s="1">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="F48" s="1">
-        <f>E48/C48</f>
+        <f t="shared" si="6"/>
         <v>4.8600883652430045E-2</v>
       </c>
       <c r="G48">
-        <f>A48*E48</f>
+        <f t="shared" si="7"/>
         <v>62841.207000000002</v>
       </c>
       <c r="H48">
@@ -2093,22 +2096,22 @@
         <v>0.316</v>
       </c>
       <c r="C49" s="3">
-        <f>1-B49</f>
+        <f t="shared" si="4"/>
         <v>0.68399999999999994</v>
       </c>
       <c r="D49">
-        <f>A49*C49</f>
+        <f t="shared" si="5"/>
         <v>1264425.2999999998</v>
       </c>
       <c r="E49" s="1">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="F49" s="1">
-        <f>E49/C49</f>
+        <f t="shared" si="6"/>
         <v>5.1169590643274865E-2</v>
       </c>
       <c r="G49">
-        <f>A49*E49</f>
+        <f t="shared" si="7"/>
         <v>64700.125000000007</v>
       </c>
       <c r="H49">
@@ -2126,22 +2129,22 @@
         <v>0.30599999999999999</v>
       </c>
       <c r="C50" s="3">
-        <f>1-B50</f>
+        <f t="shared" si="4"/>
         <v>0.69399999999999995</v>
       </c>
       <c r="D50">
-        <f>A50*C50</f>
+        <f t="shared" si="5"/>
         <v>1226383.362</v>
       </c>
       <c r="E50" s="1">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="F50" s="1">
-        <f>E50/C50</f>
+        <f t="shared" si="6"/>
         <v>6.1959654178674349E-2</v>
       </c>
       <c r="G50">
-        <f>A50*E50</f>
+        <f t="shared" si="7"/>
         <v>75986.28899999999</v>
       </c>
       <c r="H50">
@@ -2159,22 +2162,22 @@
         <v>0.30099999999999999</v>
       </c>
       <c r="C51" s="3">
-        <f>1-B51</f>
+        <f t="shared" si="4"/>
         <v>0.69900000000000007</v>
       </c>
       <c r="D51">
-        <f>A51*C51</f>
+        <f t="shared" si="5"/>
         <v>1249026.324</v>
       </c>
       <c r="E51" s="1">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="F51" s="1">
-        <f>E51/C51</f>
+        <f t="shared" si="6"/>
         <v>7.0100143061516448E-2</v>
       </c>
       <c r="G51">
-        <f>A51*E51</f>
+        <f t="shared" si="7"/>
         <v>87556.923999999999</v>
       </c>
       <c r="H51">
@@ -2192,22 +2195,22 @@
         <v>0.29599999999999999</v>
       </c>
       <c r="C52" s="3">
-        <f>1-B52</f>
+        <f t="shared" si="4"/>
         <v>0.70399999999999996</v>
       </c>
       <c r="D52">
-        <f>A52*C52</f>
+        <f t="shared" si="5"/>
         <v>1219611.7119999998</v>
       </c>
       <c r="E52" s="1">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="F52" s="1">
-        <f>E52/C52</f>
+        <f t="shared" si="6"/>
         <v>7.6704545454545456E-2</v>
       </c>
       <c r="G52">
-        <f>A52*E52</f>
+        <f t="shared" si="7"/>
         <v>93549.762000000002</v>
       </c>
       <c r="H52">
@@ -2225,22 +2228,22 @@
         <v>0.28199999999999997</v>
       </c>
       <c r="C53" s="3">
-        <f>1-B53</f>
+        <f t="shared" si="4"/>
         <v>0.71799999999999997</v>
       </c>
       <c r="D53">
-        <f>A53*C53</f>
+        <f t="shared" si="5"/>
         <v>1217771.0799999998</v>
       </c>
       <c r="E53" s="1">
         <v>5.5E-2</v>
       </c>
       <c r="F53" s="1">
-        <f>E53/C53</f>
+        <f t="shared" si="6"/>
         <v>7.660167130919221E-2</v>
       </c>
       <c r="G53">
-        <f>A53*E53</f>
+        <f t="shared" si="7"/>
         <v>93283.3</v>
       </c>
       <c r="H53">
@@ -2258,22 +2261,22 @@
         <v>0.28399999999999997</v>
       </c>
       <c r="C54" s="3">
-        <f>1-B54</f>
+        <f t="shared" si="4"/>
         <v>0.71599999999999997</v>
       </c>
       <c r="D54">
-        <f>A54*C54</f>
+        <f t="shared" si="5"/>
         <v>1177912.3640000001</v>
       </c>
       <c r="E54" s="1">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="F54" s="1">
-        <f>E54/C54</f>
+        <f t="shared" si="6"/>
         <v>6.8435754189944145E-2</v>
       </c>
       <c r="G54">
-        <f>A54*E54</f>
+        <f t="shared" si="7"/>
         <v>80611.320999999996</v>
       </c>
       <c r="H54">
@@ -2291,22 +2294,22 @@
         <v>0.27400000000000002</v>
       </c>
       <c r="C55" s="3">
-        <f>1-B55</f>
+        <f t="shared" si="4"/>
         <v>0.72599999999999998</v>
       </c>
       <c r="D55">
-        <f>A55*C55</f>
+        <f t="shared" si="5"/>
         <v>1166263.098</v>
       </c>
       <c r="E55" s="1">
         <v>3.1E-2</v>
       </c>
       <c r="F55" s="1">
-        <f>E55/C55</f>
+        <f t="shared" si="6"/>
         <v>4.2699724517906337E-2</v>
       </c>
       <c r="G55">
-        <f>A55*E55</f>
+        <f t="shared" si="7"/>
         <v>49799.112999999998</v>
       </c>
       <c r="H55">
@@ -2324,22 +2327,22 @@
         <v>0.314</v>
       </c>
       <c r="C56" s="8">
-        <f>1-B56</f>
+        <f t="shared" si="4"/>
         <v>0.68599999999999994</v>
       </c>
       <c r="D56" s="6">
-        <f>A56*C56</f>
+        <f t="shared" si="5"/>
         <v>1114942.0799999998</v>
       </c>
       <c r="E56" s="7">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="F56" s="7">
-        <f>E56/C56</f>
+        <f t="shared" si="6"/>
         <v>4.8104956268221581E-2</v>
       </c>
       <c r="G56" s="6">
-        <f>A56*E56</f>
+        <f t="shared" si="7"/>
         <v>53634.240000000005</v>
       </c>
       <c r="H56" s="6">
@@ -2357,22 +2360,22 @@
         <v>0.40500000000000003</v>
       </c>
       <c r="C57" s="3">
-        <f>1-B57</f>
+        <f t="shared" si="4"/>
         <v>0.59499999999999997</v>
       </c>
       <c r="D57">
-        <f>A57*C57</f>
+        <f t="shared" si="5"/>
         <v>751786.66499999992</v>
       </c>
       <c r="E57" s="1">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F57" s="1">
-        <f>E57/C57</f>
+        <f t="shared" si="6"/>
         <v>4.3697478991596636E-2</v>
       </c>
       <c r="G57">
-        <f>A57*E57</f>
+        <f t="shared" si="7"/>
         <v>32851.182000000001</v>
       </c>
       <c r="H57">
@@ -2390,22 +2393,22 @@
         <v>0.41899999999999998</v>
       </c>
       <c r="C58" s="3">
-        <f>1-B58</f>
+        <f t="shared" si="4"/>
         <v>0.58099999999999996</v>
       </c>
       <c r="D58">
-        <f>A58*C58</f>
+        <f t="shared" si="5"/>
         <v>714597.46399999992</v>
       </c>
       <c r="E58" s="1">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="F58" s="1">
-        <f>E58/C58</f>
+        <f t="shared" si="6"/>
         <v>4.8192771084337352E-2</v>
       </c>
       <c r="G58">
-        <f>A58*E58</f>
+        <f t="shared" si="7"/>
         <v>34438.432000000001</v>
       </c>
       <c r="H58">
@@ -2423,22 +2426,22 @@
         <v>0.43099999999999999</v>
       </c>
       <c r="C59" s="3">
-        <f>1-B59</f>
+        <f t="shared" si="4"/>
         <v>0.56899999999999995</v>
       </c>
       <c r="D59">
-        <f>A59*C59</f>
+        <f t="shared" si="5"/>
         <v>666801.99599999993</v>
       </c>
       <c r="E59" s="1">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="F59" s="1">
-        <f>E59/C59</f>
+        <f t="shared" si="6"/>
         <v>5.7996485061511428E-2</v>
       </c>
       <c r="G59">
-        <f>A59*E59</f>
+        <f t="shared" si="7"/>
         <v>38672.171999999999</v>
       </c>
       <c r="H59">
@@ -2456,22 +2459,22 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="C60" s="3">
-        <f>1-B60</f>
+        <f t="shared" si="4"/>
         <v>0.58499999999999996</v>
       </c>
       <c r="D60">
-        <f>A60*C60</f>
+        <f t="shared" si="5"/>
         <v>659076.21</v>
       </c>
       <c r="E60" s="2">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="F60" s="1">
-        <f>E60/C60</f>
+        <f t="shared" si="6"/>
         <v>7.521367521367521E-2</v>
       </c>
       <c r="G60">
-        <f>A60*E60</f>
+        <f t="shared" si="7"/>
         <v>49571.543999999994</v>
       </c>
       <c r="H60">
@@ -2489,22 +2492,22 @@
         <v>0.43099999999999999</v>
       </c>
       <c r="C61" s="3">
-        <f>1-B61</f>
+        <f t="shared" si="4"/>
         <v>0.56899999999999995</v>
       </c>
       <c r="D61">
-        <f>A61*C61</f>
+        <f t="shared" si="5"/>
         <v>628013.26599999995</v>
       </c>
       <c r="E61" s="1">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="F61" s="1">
-        <f>E61/C61</f>
+        <f t="shared" si="6"/>
         <v>8.9630931458699478E-2</v>
       </c>
       <c r="G61">
-        <f>A61*E61</f>
+        <f t="shared" si="7"/>
         <v>56289.413999999997</v>
       </c>
       <c r="H61">
@@ -2522,22 +2525,22 @@
         <v>0.41099999999999998</v>
       </c>
       <c r="C62" s="3">
-        <f>1-B62</f>
+        <f t="shared" si="4"/>
         <v>0.58899999999999997</v>
       </c>
       <c r="D62">
-        <f>A62*C62</f>
+        <f t="shared" si="5"/>
         <v>631689.54200000002</v>
       </c>
       <c r="E62" s="1">
         <v>6.3E-2</v>
       </c>
       <c r="F62" s="1">
-        <f>E62/C62</f>
+        <f t="shared" si="6"/>
         <v>0.1069609507640068</v>
       </c>
       <c r="G62">
-        <f>A62*E62</f>
+        <f t="shared" si="7"/>
         <v>67566.114000000001</v>
       </c>
       <c r="H62">
@@ -2555,22 +2558,22 @@
         <v>0.42099999999999999</v>
       </c>
       <c r="C63" s="3">
-        <f>1-B63</f>
+        <f t="shared" si="4"/>
         <v>0.57899999999999996</v>
       </c>
       <c r="D63">
-        <f>A63*C63</f>
+        <f t="shared" si="5"/>
         <v>610646.98199999996</v>
       </c>
       <c r="E63" s="1">
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="F63" s="1">
-        <f>E63/C63</f>
+        <f t="shared" si="6"/>
         <v>0.13298791018998274</v>
       </c>
       <c r="G63">
-        <f>A63*E63</f>
+        <f t="shared" si="7"/>
         <v>81208.665999999997</v>
       </c>
       <c r="H63">
@@ -2588,22 +2591,22 @@
         <v>0.41899999999999998</v>
       </c>
       <c r="C64" s="3">
-        <f>1-B64</f>
+        <f t="shared" si="4"/>
         <v>0.58099999999999996</v>
       </c>
       <c r="D64">
-        <f>A64*C64</f>
+        <f t="shared" si="5"/>
         <v>615894.27899999998</v>
       </c>
       <c r="E64" s="1">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="F64" s="1">
-        <f>E64/C64</f>
+        <f t="shared" si="6"/>
         <v>0.14457831325301207</v>
       </c>
       <c r="G64">
-        <f>A64*E64</f>
+        <f t="shared" si="7"/>
         <v>89044.956000000006</v>
       </c>
       <c r="H64">
@@ -2621,22 +2624,22 @@
         <v>0.41699999999999998</v>
       </c>
       <c r="C65" s="3">
-        <f>1-B65</f>
+        <f t="shared" si="4"/>
         <v>0.58299999999999996</v>
       </c>
       <c r="D65">
-        <f>A65*C65</f>
+        <f t="shared" si="5"/>
         <v>557351.49800000002</v>
       </c>
       <c r="E65" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F65" s="1">
-        <f>E65/C65</f>
+        <f t="shared" si="6"/>
         <v>0.1200686106346484</v>
       </c>
       <c r="G65">
-        <f>A65*E65</f>
+        <f t="shared" si="7"/>
         <v>66920.420000000013</v>
       </c>
       <c r="H65">
@@ -2654,22 +2657,22 @@
         <v>0.42599999999999999</v>
       </c>
       <c r="C66" s="3">
-        <f>1-B66</f>
+        <f t="shared" ref="C66:C97" si="8">1-B66</f>
         <v>0.57400000000000007</v>
       </c>
       <c r="D66">
-        <f>A66*C66</f>
+        <f t="shared" ref="D66:D97" si="9">A66*C66</f>
         <v>541314.14400000009</v>
       </c>
       <c r="E66" s="1">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="F66" s="1">
-        <f>E66/C66</f>
+        <f t="shared" ref="F66:F97" si="10">E66/C66</f>
         <v>6.271777003484319E-2</v>
       </c>
       <c r="G66">
-        <f>A66*E66</f>
+        <f t="shared" ref="G66:G97" si="11">A66*E66</f>
         <v>33950.015999999996</v>
       </c>
       <c r="H66">
@@ -2687,22 +2690,22 @@
         <v>0.434</v>
       </c>
       <c r="C67" s="8">
-        <f>1-B67</f>
+        <f t="shared" si="8"/>
         <v>0.56600000000000006</v>
       </c>
       <c r="D67" s="6">
-        <f>A67*C67</f>
+        <f t="shared" si="9"/>
         <v>537032.6860000001</v>
       </c>
       <c r="E67" s="7">
         <v>2.7E-2</v>
       </c>
       <c r="F67" s="7">
-        <f>E67/C67</f>
+        <f t="shared" si="10"/>
         <v>4.7703180212014126E-2</v>
       </c>
       <c r="G67" s="6">
-        <f>A67*E67</f>
+        <f t="shared" si="11"/>
         <v>25618.167000000001</v>
       </c>
       <c r="H67" s="6">
@@ -2720,22 +2723,22 @@
         <v>0.308</v>
       </c>
       <c r="C68" s="3">
-        <f>1-B68</f>
+        <f t="shared" si="8"/>
         <v>0.69199999999999995</v>
       </c>
       <c r="D68">
-        <f>A68*C68</f>
+        <f t="shared" si="9"/>
         <v>441351.37199999997</v>
       </c>
       <c r="E68" s="1">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F68" s="1">
-        <f>E68/C68</f>
+        <f t="shared" si="10"/>
         <v>6.936416184971099E-2</v>
       </c>
       <c r="G68">
-        <f>A68*E68</f>
+        <f t="shared" si="11"/>
         <v>30613.968000000001</v>
       </c>
       <c r="H68">
@@ -2753,22 +2756,22 @@
         <v>0.30399999999999999</v>
       </c>
       <c r="C69" s="3">
-        <f>1-B69</f>
+        <f t="shared" si="8"/>
         <v>0.69599999999999995</v>
       </c>
       <c r="D69">
-        <f>A69*C69</f>
+        <f t="shared" si="9"/>
         <v>440025.81599999999</v>
       </c>
       <c r="E69" s="2">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="F69" s="1">
-        <f>E69/C69</f>
+        <f t="shared" si="10"/>
         <v>7.3275862068965511E-2</v>
       </c>
       <c r="G69">
-        <f>A69*E69</f>
+        <f t="shared" si="11"/>
         <v>32243.270999999997</v>
       </c>
       <c r="H69">
@@ -2786,22 +2789,22 @@
         <v>0.28699999999999998</v>
       </c>
       <c r="C70" s="3">
-        <f>1-B70</f>
+        <f t="shared" si="8"/>
         <v>0.71300000000000008</v>
       </c>
       <c r="D70">
-        <f>A70*C70</f>
+        <f t="shared" si="9"/>
         <v>458609.44300000003</v>
       </c>
       <c r="E70" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="F70" s="1">
-        <f>E70/C70</f>
+        <f t="shared" si="10"/>
         <v>8.9761570827489479E-2</v>
       </c>
       <c r="G70">
-        <f>A70*E70</f>
+        <f t="shared" si="11"/>
         <v>41165.504000000001</v>
       </c>
       <c r="H70">
@@ -2819,22 +2822,22 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="C71" s="3">
-        <f>1-B71</f>
+        <f t="shared" si="8"/>
         <v>0.71399999999999997</v>
       </c>
       <c r="D71">
-        <f>A71*C71</f>
+        <f t="shared" si="9"/>
         <v>425947.41</v>
       </c>
       <c r="E71" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F71" s="1">
-        <f>E71/C71</f>
+        <f t="shared" si="10"/>
         <v>9.8039215686274522E-2</v>
       </c>
       <c r="G71">
-        <f>A71*E71</f>
+        <f t="shared" si="11"/>
         <v>41759.550000000003</v>
       </c>
       <c r="H71">
@@ -2852,22 +2855,22 @@
         <v>0.29599999999999999</v>
       </c>
       <c r="C72" s="3">
-        <f>1-B72</f>
+        <f t="shared" si="8"/>
         <v>0.70399999999999996</v>
       </c>
       <c r="D72">
-        <f>A72*C72</f>
+        <f t="shared" si="9"/>
         <v>396946.88</v>
       </c>
       <c r="E72" s="1">
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="F72" s="1">
-        <f>E72/C72</f>
+        <f t="shared" si="10"/>
         <v>0.12357954545454546</v>
       </c>
       <c r="G72">
-        <f>A72*E72</f>
+        <f t="shared" si="11"/>
         <v>49054.514999999999</v>
       </c>
       <c r="H72">
@@ -2885,22 +2888,22 @@
         <v>0.29299999999999998</v>
       </c>
       <c r="C73" s="3">
-        <f>1-B73</f>
+        <f t="shared" si="8"/>
         <v>0.70700000000000007</v>
       </c>
       <c r="D73">
-        <f>A73*C73</f>
+        <f t="shared" si="9"/>
         <v>403452.37800000003</v>
       </c>
       <c r="E73" s="1">
         <v>0.106</v>
       </c>
       <c r="F73" s="1">
-        <f>E73/C73</f>
+        <f t="shared" si="10"/>
         <v>0.14992927864214992</v>
       </c>
       <c r="G73">
-        <f>A73*E73</f>
+        <f t="shared" si="11"/>
         <v>60489.324000000001</v>
       </c>
       <c r="H73">
@@ -2918,22 +2921,22 @@
         <v>0.29099999999999998</v>
       </c>
       <c r="C74" s="3">
-        <f>1-B74</f>
+        <f t="shared" si="8"/>
         <v>0.70900000000000007</v>
       </c>
       <c r="D74">
-        <f>A74*C74</f>
+        <f t="shared" si="9"/>
         <v>394074.25300000003</v>
       </c>
       <c r="E74" s="1">
         <v>0.10199999999999999</v>
       </c>
       <c r="F74" s="1">
-        <f>E74/C74</f>
+        <f t="shared" si="10"/>
         <v>0.14386459802538784</v>
       </c>
       <c r="G74">
-        <f>A74*E74</f>
+        <f t="shared" si="11"/>
         <v>56693.333999999995</v>
       </c>
       <c r="H74">
@@ -2951,22 +2954,22 @@
         <v>0.29099999999999998</v>
       </c>
       <c r="C75" s="3">
-        <f>1-B75</f>
+        <f t="shared" si="8"/>
         <v>0.70900000000000007</v>
       </c>
       <c r="D75">
-        <f>A75*C75</f>
+        <f t="shared" si="9"/>
         <v>390204.53100000002</v>
       </c>
       <c r="E75" s="1">
         <v>0.112</v>
       </c>
       <c r="F75" s="1">
-        <f>E75/C75</f>
+        <f t="shared" si="10"/>
         <v>0.15796897038081803</v>
       </c>
       <c r="G75">
-        <f>A75*E75</f>
+        <f t="shared" si="11"/>
         <v>61640.207999999999</v>
       </c>
       <c r="H75">
@@ -2984,22 +2987,22 @@
         <v>0.27500000000000002</v>
       </c>
       <c r="C76" s="3">
-        <f>1-B76</f>
+        <f t="shared" si="8"/>
         <v>0.72499999999999998</v>
       </c>
       <c r="D76">
-        <f>A76*C76</f>
+        <f t="shared" si="9"/>
         <v>365243.39999999997</v>
       </c>
       <c r="E76" s="1">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="F76" s="1">
-        <f>E76/C76</f>
+        <f t="shared" si="10"/>
         <v>0.12689655172413794</v>
       </c>
       <c r="G76">
-        <f>A76*E76</f>
+        <f t="shared" si="11"/>
         <v>46348.127999999997</v>
       </c>
       <c r="H76">
@@ -3017,22 +3020,22 @@
         <v>0.24299999999999999</v>
       </c>
       <c r="C77" s="3">
-        <f>1-B77</f>
+        <f t="shared" si="8"/>
         <v>0.75700000000000001</v>
       </c>
       <c r="D77">
-        <f>A77*C77</f>
+        <f t="shared" si="9"/>
         <v>378848.22000000003</v>
       </c>
       <c r="E77" s="1">
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F77" s="1">
-        <f>E77/C77</f>
+        <f t="shared" si="10"/>
         <v>9.6433289299867886E-2</v>
       </c>
       <c r="G77">
-        <f>A77*E77</f>
+        <f t="shared" si="11"/>
         <v>36533.579999999994</v>
       </c>
       <c r="H77">
@@ -3050,22 +3053,22 @@
         <v>0.26500000000000001</v>
       </c>
       <c r="C78" s="8">
-        <f>1-B78</f>
+        <f t="shared" si="8"/>
         <v>0.73499999999999999</v>
       </c>
       <c r="D78" s="6">
-        <f>A78*C78</f>
+        <f t="shared" si="9"/>
         <v>364232.19</v>
       </c>
       <c r="E78" s="7">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="F78" s="7">
-        <f>E78/C78</f>
+        <f t="shared" si="10"/>
         <v>8.2993197278911565E-2</v>
       </c>
       <c r="G78" s="6">
-        <f>A78*E78</f>
+        <f t="shared" si="11"/>
         <v>30228.793999999998</v>
       </c>
       <c r="H78" s="6">
@@ -3083,22 +3086,22 @@
         <v>0.34499999999999997</v>
       </c>
       <c r="C79" s="3">
-        <f>1-B79</f>
+        <f t="shared" si="8"/>
         <v>0.65500000000000003</v>
       </c>
       <c r="D79">
-        <f>A79*C79</f>
+        <f t="shared" si="9"/>
         <v>855152.28</v>
       </c>
       <c r="E79" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F79" s="1">
-        <f>E79/C79</f>
+        <f t="shared" si="10"/>
         <v>3.358778625954198E-2</v>
       </c>
       <c r="G79">
-        <f>A79*E79</f>
+        <f t="shared" si="11"/>
         <v>28722.671999999999</v>
       </c>
       <c r="H79">
@@ -3116,22 +3119,22 @@
         <v>0.33400000000000002</v>
       </c>
       <c r="C80" s="3">
-        <f>1-B80</f>
+        <f t="shared" si="8"/>
         <v>0.66599999999999993</v>
       </c>
       <c r="D80">
-        <f>A80*C80</f>
+        <f t="shared" si="9"/>
         <v>873109.34999999986</v>
       </c>
       <c r="E80" s="1">
         <v>2.7E-2</v>
       </c>
       <c r="F80" s="1">
-        <f>E80/C80</f>
+        <f t="shared" si="10"/>
         <v>4.0540540540540543E-2</v>
       </c>
       <c r="G80">
-        <f>A80*E80</f>
+        <f t="shared" si="11"/>
         <v>35396.324999999997</v>
       </c>
       <c r="H80">
@@ -3149,22 +3152,22 @@
         <v>0.33700000000000002</v>
       </c>
       <c r="C81" s="3">
-        <f>1-B81</f>
+        <f t="shared" si="8"/>
         <v>0.66300000000000003</v>
       </c>
       <c r="D81">
-        <f>A81*C81</f>
+        <f t="shared" si="9"/>
         <v>835185.0780000001</v>
       </c>
       <c r="E81" s="1">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="F81" s="1">
-        <f>E81/C81</f>
+        <f t="shared" si="10"/>
         <v>4.2232277526395169E-2</v>
       </c>
       <c r="G81">
-        <f>A81*E81</f>
+        <f t="shared" si="11"/>
         <v>35271.768000000004</v>
       </c>
       <c r="H81">
@@ -3182,22 +3185,22 @@
         <v>0.32700000000000001</v>
       </c>
       <c r="C82" s="3">
-        <f>1-B82</f>
+        <f t="shared" si="8"/>
         <v>0.67300000000000004</v>
       </c>
       <c r="D82">
-        <f>A82*C82</f>
+        <f t="shared" si="9"/>
         <v>843656.64800000004</v>
       </c>
       <c r="E82" s="1">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="F82" s="1">
-        <f>E82/C82</f>
+        <f t="shared" si="10"/>
         <v>4.7548291233283801E-2</v>
       </c>
       <c r="G82">
-        <f>A82*E82</f>
+        <f t="shared" si="11"/>
         <v>40114.432000000001</v>
       </c>
       <c r="H82">
@@ -3215,22 +3218,22 @@
         <v>0.32100000000000001</v>
       </c>
       <c r="C83" s="3">
-        <f>1-B83</f>
+        <f t="shared" si="8"/>
         <v>0.67900000000000005</v>
       </c>
       <c r="D83">
-        <f>A83*C83</f>
+        <f t="shared" si="9"/>
         <v>839814.3600000001</v>
       </c>
       <c r="E83" s="1">
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="F83" s="1">
-        <f>E83/C83</f>
+        <f t="shared" si="10"/>
         <v>6.0382916053019146E-2</v>
       </c>
       <c r="G83">
-        <f>A83*E83</f>
+        <f t="shared" si="11"/>
         <v>50710.44</v>
       </c>
       <c r="H83">
@@ -3248,22 +3251,22 @@
         <v>0.311</v>
       </c>
       <c r="C84" s="3">
-        <f>1-B84</f>
+        <f t="shared" si="8"/>
         <v>0.68900000000000006</v>
       </c>
       <c r="D84">
-        <f>A84*C84</f>
+        <f t="shared" si="9"/>
         <v>841038.87400000007</v>
       </c>
       <c r="E84" s="2">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F84" s="1">
-        <f>E84/C84</f>
+        <f t="shared" si="10"/>
         <v>6.966618287373004E-2</v>
       </c>
       <c r="G84">
-        <f>A84*E84</f>
+        <f t="shared" si="11"/>
         <v>58591.968000000001</v>
       </c>
       <c r="H84">
@@ -3281,22 +3284,22 @@
         <v>0.32</v>
       </c>
       <c r="C85" s="3">
-        <f>1-B85</f>
+        <f t="shared" si="8"/>
         <v>0.67999999999999994</v>
       </c>
       <c r="D85">
-        <f>A85*C85</f>
+        <f t="shared" si="9"/>
         <v>831965.72</v>
       </c>
       <c r="E85" s="1">
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="F85" s="1">
-        <f>E85/C85</f>
+        <f t="shared" si="10"/>
         <v>8.6764705882352938E-2</v>
       </c>
       <c r="G85">
-        <f>A85*E85</f>
+        <f t="shared" si="11"/>
         <v>72185.260999999999</v>
       </c>
       <c r="H85">
@@ -3314,22 +3317,22 @@
         <v>0.312</v>
       </c>
       <c r="C86" s="3">
-        <f>1-B86</f>
+        <f t="shared" si="8"/>
         <v>0.68799999999999994</v>
       </c>
       <c r="D86">
-        <f>A86*C86</f>
+        <f t="shared" si="9"/>
         <v>822045.7919999999</v>
       </c>
       <c r="E86" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="F86" s="1">
-        <f>E86/C86</f>
+        <f t="shared" si="10"/>
         <v>9.3023255813953501E-2</v>
       </c>
       <c r="G86">
-        <f>A86*E86</f>
+        <f t="shared" si="11"/>
         <v>76469.376000000004</v>
       </c>
       <c r="H86">
@@ -3347,22 +3350,22 @@
         <v>0.30599999999999999</v>
       </c>
       <c r="C87" s="3">
-        <f>1-B87</f>
+        <f t="shared" si="8"/>
         <v>0.69399999999999995</v>
       </c>
       <c r="D87">
-        <f>A87*C87</f>
+        <f t="shared" si="9"/>
         <v>771085.35599999991</v>
       </c>
       <c r="E87" s="1">
         <v>0.06</v>
       </c>
       <c r="F87" s="1">
-        <f>E87/C87</f>
+        <f t="shared" si="10"/>
         <v>8.645533141210375E-2</v>
       </c>
       <c r="G87">
-        <f>A87*E87</f>
+        <f t="shared" si="11"/>
         <v>66664.44</v>
       </c>
       <c r="H87">
@@ -3380,22 +3383,22 @@
         <v>0.28399999999999997</v>
       </c>
       <c r="C88" s="3">
-        <f>1-B88</f>
+        <f t="shared" si="8"/>
         <v>0.71599999999999997</v>
       </c>
       <c r="D88">
-        <f>A88*C88</f>
+        <f t="shared" si="9"/>
         <v>789131.52399999998</v>
       </c>
       <c r="E88" s="1">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="F88" s="1">
-        <f>E88/C88</f>
+        <f t="shared" si="10"/>
         <v>4.8882681564245814E-2</v>
       </c>
       <c r="G88">
-        <f>A88*E88</f>
+        <f t="shared" si="11"/>
         <v>38574.865000000005</v>
       </c>
       <c r="H88">
@@ -3413,22 +3416,22 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="C89" s="8">
-        <f>1-B89</f>
+        <f t="shared" si="8"/>
         <v>0.66199999999999992</v>
       </c>
       <c r="D89" s="6">
-        <f>A89*C89</f>
+        <f t="shared" si="9"/>
         <v>704072.08599999989</v>
       </c>
       <c r="E89" s="7">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F89" s="7">
-        <f>E89/C89</f>
+        <f t="shared" si="10"/>
         <v>7.2507552870090641E-2</v>
       </c>
       <c r="G89" s="6">
-        <f>A89*E89</f>
+        <f t="shared" si="11"/>
         <v>51050.544000000002</v>
       </c>
       <c r="H89" s="6">
@@ -3446,22 +3449,22 @@
         <v>0.32600000000000001</v>
       </c>
       <c r="C90" s="3">
-        <f>1-B90</f>
+        <f t="shared" si="8"/>
         <v>0.67399999999999993</v>
       </c>
       <c r="D90">
-        <f>A90*C90</f>
+        <f t="shared" si="9"/>
         <v>733755.49199999997</v>
       </c>
       <c r="E90" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="F90" s="1">
-        <f>E90/C90</f>
+        <f t="shared" si="10"/>
         <v>9.7922848664688436E-2</v>
       </c>
       <c r="G90">
-        <f>A90*E90</f>
+        <f t="shared" si="11"/>
         <v>71851.428</v>
       </c>
       <c r="H90">
@@ -3479,22 +3482,22 @@
         <v>0.33700000000000002</v>
       </c>
       <c r="C91" s="3">
-        <f>1-B91</f>
+        <f t="shared" si="8"/>
         <v>0.66300000000000003</v>
       </c>
       <c r="D91">
-        <f>A91*C91</f>
+        <f t="shared" si="9"/>
         <v>671998.89900000009</v>
       </c>
       <c r="E91" s="1">
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="F91" s="1">
-        <f>E91/C91</f>
+        <f t="shared" si="10"/>
         <v>7.8431372549019607E-2</v>
       </c>
       <c r="G91">
-        <f>A91*E91</f>
+        <f t="shared" si="11"/>
         <v>52705.795999999995</v>
       </c>
       <c r="H91">
@@ -3512,22 +3515,22 @@
         <v>0.34300000000000003</v>
       </c>
       <c r="C92" s="3">
-        <f>1-B92</f>
+        <f t="shared" si="8"/>
         <v>0.65700000000000003</v>
       </c>
       <c r="D92">
-        <f>A92*C92</f>
+        <f t="shared" si="9"/>
         <v>657310.76100000006</v>
       </c>
       <c r="E92" s="1">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="F92" s="1">
-        <f>E92/C92</f>
+        <f t="shared" si="10"/>
         <v>8.5235920852359204E-2</v>
       </c>
       <c r="G92">
-        <f>A92*E92</f>
+        <f t="shared" si="11"/>
         <v>56026.487999999998</v>
       </c>
       <c r="H92">
@@ -3545,22 +3548,22 @@
         <v>0.34399999999999997</v>
       </c>
       <c r="C93" s="3">
-        <f>1-B93</f>
+        <f t="shared" si="8"/>
         <v>0.65600000000000003</v>
       </c>
       <c r="D93">
-        <f>A93*C93</f>
+        <f t="shared" si="9"/>
         <v>613806.08000000007</v>
       </c>
       <c r="E93" s="1">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="F93" s="1">
-        <f>E93/C93</f>
+        <f t="shared" si="10"/>
         <v>9.298780487804878E-2</v>
       </c>
       <c r="G93">
-        <f>A93*E93</f>
+        <f t="shared" si="11"/>
         <v>57076.479999999996</v>
       </c>
       <c r="H93">
@@ -3578,22 +3581,22 @@
         <v>0.32800000000000001</v>
       </c>
       <c r="C94" s="3">
-        <f>1-B94</f>
+        <f t="shared" si="8"/>
         <v>0.67199999999999993</v>
       </c>
       <c r="D94">
-        <f>A94*C94</f>
+        <f t="shared" si="9"/>
         <v>625625.95199999993</v>
       </c>
       <c r="E94" s="1">
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="F94" s="1">
-        <f>E94/C94</f>
+        <f t="shared" si="10"/>
         <v>0.11458333333333334</v>
       </c>
       <c r="G94">
-        <f>A94*E94</f>
+        <f t="shared" si="11"/>
         <v>71686.307000000001</v>
       </c>
       <c r="H94">
@@ -3611,22 +3614,22 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="C95" s="3">
-        <f>1-B95</f>
+        <f t="shared" si="8"/>
         <v>0.66700000000000004</v>
       </c>
       <c r="D95">
-        <f>A95*C95</f>
+        <f t="shared" si="9"/>
         <v>600540.78700000001</v>
       </c>
       <c r="E95" s="1">
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="F95" s="1">
-        <f>E95/C95</f>
+        <f t="shared" si="10"/>
         <v>0.12893553223388304</v>
       </c>
       <c r="G95">
-        <f>A95*E95</f>
+        <f t="shared" si="11"/>
         <v>77431.045999999988</v>
       </c>
       <c r="H95">
@@ -3644,22 +3647,22 @@
         <v>0.33100000000000002</v>
       </c>
       <c r="C96" s="3">
-        <f>1-B96</f>
+        <f t="shared" si="8"/>
         <v>0.66900000000000004</v>
       </c>
       <c r="D96">
-        <f>A96*C96</f>
+        <f t="shared" si="9"/>
         <v>563359.54800000007</v>
       </c>
       <c r="E96" s="1">
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="F96" s="1">
-        <f>E96/C96</f>
+        <f t="shared" si="10"/>
         <v>0.13004484304932734</v>
       </c>
       <c r="G96">
-        <f>A96*E96</f>
+        <f t="shared" si="11"/>
         <v>73262.004000000001</v>
       </c>
       <c r="H96">
@@ -3677,22 +3680,22 @@
         <v>0.32900000000000001</v>
       </c>
       <c r="C97" s="3">
-        <f>1-B97</f>
+        <f t="shared" si="8"/>
         <v>0.67100000000000004</v>
       </c>
       <c r="D97">
-        <f>A97*C97</f>
+        <f t="shared" si="9"/>
         <v>557647.97000000009</v>
       </c>
       <c r="E97" s="1">
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="F97" s="1">
-        <f>E97/C97</f>
+        <f t="shared" si="10"/>
         <v>0.13114754098360654</v>
       </c>
       <c r="G97">
-        <f>A97*E97</f>
+        <f t="shared" si="11"/>
         <v>73134.159999999989</v>
       </c>
       <c r="H97">
@@ -3710,22 +3713,22 @@
         <v>0.32300000000000001</v>
       </c>
       <c r="C98" s="3">
-        <f>1-B98</f>
+        <f t="shared" ref="C98:C122" si="12">1-B98</f>
         <v>0.67700000000000005</v>
       </c>
       <c r="D98">
-        <f>A98*C98</f>
+        <f t="shared" ref="D98:D111" si="13">A98*C98</f>
         <v>509169.66900000005</v>
       </c>
       <c r="E98" s="1">
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="F98" s="1">
-        <f>E98/C98</f>
+        <f t="shared" ref="F98:F111" si="14">E98/C98</f>
         <v>0.11964549483013294</v>
       </c>
       <c r="G98">
-        <f>A98*E98</f>
+        <f t="shared" ref="G98:G111" si="15">A98*E98</f>
         <v>60919.857000000004</v>
       </c>
       <c r="H98">
@@ -3743,22 +3746,22 @@
         <v>0.31900000000000001</v>
       </c>
       <c r="C99" s="3">
-        <f>1-B99</f>
+        <f t="shared" si="12"/>
         <v>0.68100000000000005</v>
       </c>
       <c r="D99">
-        <f>A99*C99</f>
+        <f t="shared" si="13"/>
         <v>495469.72200000001</v>
       </c>
       <c r="E99" s="1">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="F99" s="1">
-        <f>E99/C99</f>
+        <f t="shared" si="14"/>
         <v>8.9574155653450796E-2</v>
       </c>
       <c r="G99">
-        <f>A99*E99</f>
+        <f t="shared" si="15"/>
         <v>44381.281999999999</v>
       </c>
       <c r="H99">
@@ -3776,22 +3779,22 @@
         <v>0.33600000000000002</v>
       </c>
       <c r="C100" s="8">
-        <f>1-B100</f>
+        <f t="shared" si="12"/>
         <v>0.66399999999999992</v>
       </c>
       <c r="D100" s="6">
-        <f>A100*C100</f>
+        <f t="shared" si="13"/>
         <v>472147.82399999996</v>
       </c>
       <c r="E100" s="7">
         <v>5.5E-2</v>
       </c>
       <c r="F100" s="7">
-        <f>E100/C100</f>
+        <f t="shared" si="14"/>
         <v>8.2831325301204822E-2</v>
       </c>
       <c r="G100" s="6">
-        <f>A100*E100</f>
+        <f t="shared" si="15"/>
         <v>39108.629999999997</v>
       </c>
       <c r="H100" s="6">
@@ -3809,22 +3812,22 @@
         <v>0.314</v>
       </c>
       <c r="C101" s="3">
-        <f>1-B101</f>
+        <f t="shared" si="12"/>
         <v>0.68599999999999994</v>
       </c>
       <c r="D101">
-        <f>A101*C101</f>
+        <f t="shared" si="13"/>
         <v>520244.56399999995</v>
       </c>
       <c r="E101" s="1">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="F101" s="1">
-        <f>E101/C101</f>
+        <f t="shared" si="14"/>
         <v>4.6647230320699715E-2</v>
       </c>
       <c r="G101">
-        <f>A101*E101</f>
+        <f t="shared" si="15"/>
         <v>24267.968000000001</v>
       </c>
       <c r="H101">
@@ -3842,22 +3845,22 @@
         <v>0.30599999999999999</v>
       </c>
       <c r="C102" s="3">
-        <f>1-B102</f>
+        <f t="shared" si="12"/>
         <v>0.69399999999999995</v>
       </c>
       <c r="D102">
-        <f>A102*C102</f>
+        <f t="shared" si="13"/>
         <v>473810.45599999995</v>
       </c>
       <c r="E102" s="1">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="F102" s="1">
-        <f>E102/C102</f>
+        <f t="shared" si="14"/>
         <v>4.7550432276657069E-2</v>
       </c>
       <c r="G102">
-        <f>A102*E102</f>
+        <f t="shared" si="15"/>
         <v>22529.892</v>
       </c>
       <c r="H102">
@@ -3875,22 +3878,22 @@
         <v>0.315</v>
       </c>
       <c r="C103" s="3">
-        <f>1-B103</f>
+        <f t="shared" si="12"/>
         <v>0.68500000000000005</v>
       </c>
       <c r="D103">
-        <f>A103*C103</f>
+        <f t="shared" si="13"/>
         <v>462358.56000000006</v>
       </c>
       <c r="E103" s="1">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="F103" s="1">
-        <f>E103/C103</f>
+        <f t="shared" si="14"/>
         <v>5.5474452554744522E-2</v>
       </c>
       <c r="G103">
-        <f>A103*E103</f>
+        <f t="shared" si="15"/>
         <v>25649.088</v>
       </c>
       <c r="H103">
@@ -3908,22 +3911,22 @@
         <v>0.312</v>
       </c>
       <c r="C104" s="3">
-        <f>1-B104</f>
+        <f t="shared" si="12"/>
         <v>0.68799999999999994</v>
       </c>
       <c r="D104">
-        <f>A104*C104</f>
+        <f t="shared" si="13"/>
         <v>471001.36</v>
       </c>
       <c r="E104" s="1">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F104" s="1">
-        <f>E104/C104</f>
+        <f t="shared" si="14"/>
         <v>6.5406976744186052E-2</v>
       </c>
       <c r="G104">
-        <f>A104*E104</f>
+        <f t="shared" si="15"/>
         <v>30806.774999999998</v>
       </c>
       <c r="H104">
@@ -3941,22 +3944,22 @@
         <v>0.3</v>
       </c>
       <c r="C105" s="3">
-        <f>1-B105</f>
+        <f t="shared" si="12"/>
         <v>0.7</v>
       </c>
       <c r="D105">
-        <f>A105*C105</f>
+        <f t="shared" si="13"/>
         <v>455325.5</v>
       </c>
       <c r="E105" s="1">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="F105" s="1">
-        <f>E105/C105</f>
+        <f t="shared" si="14"/>
         <v>7.571428571428572E-2</v>
       </c>
       <c r="G105">
-        <f>A105*E105</f>
+        <f t="shared" si="15"/>
         <v>34474.644999999997</v>
       </c>
       <c r="H105">
@@ -3974,22 +3977,22 @@
         <v>0.29299999999999998</v>
       </c>
       <c r="C106" s="3">
-        <f>1-B106</f>
+        <f t="shared" si="12"/>
         <v>0.70700000000000007</v>
       </c>
       <c r="D106">
-        <f>A106*C106</f>
+        <f t="shared" si="13"/>
         <v>459299.72200000007</v>
       </c>
       <c r="E106" s="1">
         <v>0.06</v>
       </c>
       <c r="F106" s="1">
-        <f>E106/C106</f>
+        <f t="shared" si="14"/>
         <v>8.4865629420084854E-2</v>
       </c>
       <c r="G106">
-        <f>A106*E106</f>
+        <f t="shared" si="15"/>
         <v>38978.76</v>
       </c>
       <c r="H106">
@@ -4007,22 +4010,22 @@
         <v>0.28499999999999998</v>
       </c>
       <c r="C107" s="3">
-        <f>1-B107</f>
+        <f t="shared" si="12"/>
         <v>0.71500000000000008</v>
       </c>
       <c r="D107">
-        <f>A107*C107</f>
+        <f t="shared" si="13"/>
         <v>447825.23500000004</v>
       </c>
       <c r="E107" s="1">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="F107" s="1">
-        <f>E107/C107</f>
+        <f t="shared" si="14"/>
         <v>9.5104895104895101E-2</v>
       </c>
       <c r="G107">
-        <f>A107*E107</f>
+        <f t="shared" si="15"/>
         <v>42590.372000000003</v>
       </c>
       <c r="H107">
@@ -4040,22 +4043,22 @@
         <v>0.29599999999999999</v>
       </c>
       <c r="C108" s="3">
-        <f>1-B108</f>
+        <f t="shared" si="12"/>
         <v>0.70399999999999996</v>
       </c>
       <c r="D108">
-        <f>A108*C108</f>
+        <f t="shared" si="13"/>
         <v>424610.56</v>
       </c>
       <c r="E108" s="2">
         <v>7.8E-2</v>
       </c>
       <c r="F108" s="1">
-        <f>E108/C108</f>
+        <f t="shared" si="14"/>
         <v>0.11079545454545456</v>
       </c>
       <c r="G108">
-        <f>A108*E108</f>
+        <f t="shared" si="15"/>
         <v>47044.92</v>
       </c>
       <c r="H108">
@@ -4073,22 +4076,22 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="C109" s="3">
-        <f>1-B109</f>
+        <f t="shared" si="12"/>
         <v>0.72799999999999998</v>
       </c>
       <c r="D109">
-        <f>A109*C109</f>
+        <f t="shared" si="13"/>
         <v>419165.65600000002</v>
       </c>
       <c r="E109" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="F109" s="1">
-        <f>E109/C109</f>
+        <f t="shared" si="14"/>
         <v>9.065934065934067E-2</v>
       </c>
       <c r="G109">
-        <f>A109*E109</f>
+        <f t="shared" si="15"/>
         <v>38001.281999999999</v>
       </c>
       <c r="H109">
@@ -4106,22 +4109,22 @@
         <v>0.27100000000000002</v>
       </c>
       <c r="C110" s="3">
-        <f>1-B110</f>
+        <f t="shared" si="12"/>
         <v>0.72899999999999998</v>
       </c>
       <c r="D110">
-        <f>A110*C110</f>
+        <f t="shared" si="13"/>
         <v>413715.51899999997</v>
       </c>
       <c r="E110" s="1">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F110" s="1">
-        <f>E110/C110</f>
+        <f t="shared" si="14"/>
         <v>6.1728395061728392E-2</v>
       </c>
       <c r="G110">
-        <f>A110*E110</f>
+        <f t="shared" si="15"/>
         <v>25537.994999999999</v>
       </c>
       <c r="H110">
@@ -4139,22 +4142,22 @@
         <v>0.30099999999999999</v>
       </c>
       <c r="C111" s="3">
-        <f>1-B111</f>
+        <f t="shared" si="12"/>
         <v>0.69900000000000007</v>
       </c>
       <c r="D111">
-        <f>A111*C111</f>
+        <f t="shared" si="13"/>
         <v>398744.55000000005</v>
       </c>
       <c r="E111" s="2">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="F111" s="1">
-        <f>E111/C111</f>
+        <f t="shared" si="14"/>
         <v>5.1502145922746774E-2</v>
       </c>
       <c r="G111">
-        <f>A111*E111</f>
+        <f t="shared" si="15"/>
         <v>20536.199999999997</v>
       </c>
       <c r="H111">
@@ -4162,6 +4165,369 @@
       </c>
       <c r="I111" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" s="5">
+        <v>723300</v>
+      </c>
+      <c r="B112" s="2">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="C112" s="3">
+        <f t="shared" si="12"/>
+        <v>0.71300000000000008</v>
+      </c>
+      <c r="D112">
+        <f t="shared" ref="D112" si="16">A112*C112</f>
+        <v>515712.90000000008</v>
+      </c>
+      <c r="E112" s="1">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F112" s="1">
+        <f t="shared" ref="F112" si="17">E112/C112</f>
+        <v>5.890603085553997E-2</v>
+      </c>
+      <c r="G112">
+        <f t="shared" ref="G112" si="18">A112*E112</f>
+        <v>30378.600000000002</v>
+      </c>
+      <c r="H112">
+        <v>2017</v>
+      </c>
+      <c r="I112" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" s="4">
+        <v>717207</v>
+      </c>
+      <c r="B113" s="2">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="C113" s="3">
+        <f t="shared" si="12"/>
+        <v>0.71500000000000008</v>
+      </c>
+      <c r="D113">
+        <f t="shared" ref="D113:D122" si="19">A113*C113</f>
+        <v>512803.00500000006</v>
+      </c>
+      <c r="E113" s="2">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="F113" s="1">
+        <f t="shared" ref="F113:F122" si="20">E113/C113</f>
+        <v>6.853146853146852E-2</v>
+      </c>
+      <c r="G113">
+        <f t="shared" ref="G113:G122" si="21">A113*E113</f>
+        <v>35143.143000000004</v>
+      </c>
+      <c r="H113">
+        <v>2016</v>
+      </c>
+      <c r="I113" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" s="4">
+        <v>689996</v>
+      </c>
+      <c r="B114" s="2">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="C114" s="3">
+        <f t="shared" si="12"/>
+        <v>0.70700000000000007</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="19"/>
+        <v>487827.17200000008</v>
+      </c>
+      <c r="E114" s="2">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="F114" s="1">
+        <f t="shared" si="20"/>
+        <v>8.0622347949080617E-2</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="21"/>
+        <v>39329.772000000004</v>
+      </c>
+      <c r="H114">
+        <v>2015</v>
+      </c>
+      <c r="I114" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" s="4">
+        <v>686676</v>
+      </c>
+      <c r="B115" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C115" s="3">
+        <f t="shared" si="12"/>
+        <v>0.72</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="19"/>
+        <v>494406.72</v>
+      </c>
+      <c r="E115" s="2">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="F115" s="1">
+        <f t="shared" si="20"/>
+        <v>9.4444444444444456E-2</v>
+      </c>
+      <c r="G115">
+        <f t="shared" si="21"/>
+        <v>46693.968000000001</v>
+      </c>
+      <c r="H115">
+        <v>2014</v>
+      </c>
+      <c r="I115" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" s="4">
+        <v>691163</v>
+      </c>
+      <c r="B116" s="2">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="C116" s="3">
+        <f t="shared" si="12"/>
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="19"/>
+        <v>499019.68599999999</v>
+      </c>
+      <c r="E116" s="2">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F116" s="1">
+        <f t="shared" si="20"/>
+        <v>0.10803324099722993</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="21"/>
+        <v>53910.714</v>
+      </c>
+      <c r="H116">
+        <v>2013</v>
+      </c>
+      <c r="I116" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" s="4">
+        <v>660195</v>
+      </c>
+      <c r="B117" s="2">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="C117" s="3">
+        <f t="shared" si="12"/>
+        <v>0.71300000000000008</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="19"/>
+        <v>470719.03500000003</v>
+      </c>
+      <c r="E117" s="2">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="F117" s="1">
+        <f t="shared" si="20"/>
+        <v>0.12482468443197754</v>
+      </c>
+      <c r="G117">
+        <f t="shared" si="21"/>
+        <v>58757.354999999996</v>
+      </c>
+      <c r="H117">
+        <v>2012</v>
+      </c>
+      <c r="I117" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" s="4">
+        <v>674297</v>
+      </c>
+      <c r="B118" s="2">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="C118" s="3">
+        <f t="shared" si="12"/>
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="19"/>
+        <v>493585.40399999998</v>
+      </c>
+      <c r="E118" s="2">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="F118" s="1">
+        <f t="shared" si="20"/>
+        <v>0.11885245901639344</v>
+      </c>
+      <c r="G118">
+        <f t="shared" si="21"/>
+        <v>58663.838999999993</v>
+      </c>
+      <c r="H118">
+        <v>2011</v>
+      </c>
+      <c r="I118" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" s="5">
+        <v>638172</v>
+      </c>
+      <c r="B119" s="1">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="C119" s="3">
+        <f t="shared" si="12"/>
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="19"/>
+        <v>467141.90399999998</v>
+      </c>
+      <c r="E119" s="1">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="F119" s="1">
+        <f t="shared" si="20"/>
+        <v>0.12704918032786885</v>
+      </c>
+      <c r="G119">
+        <f t="shared" si="21"/>
+        <v>59349.995999999999</v>
+      </c>
+      <c r="H119">
+        <v>2010</v>
+      </c>
+      <c r="I119" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" s="5">
+        <v>628673</v>
+      </c>
+      <c r="B120" s="2">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="C120" s="3">
+        <f t="shared" si="12"/>
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="19"/>
+        <v>480934.84500000003</v>
+      </c>
+      <c r="E120" s="2">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="F120" s="1">
+        <f t="shared" si="20"/>
+        <v>0.10980392156862745</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="21"/>
+        <v>52808.532000000007</v>
+      </c>
+      <c r="H120">
+        <v>2009</v>
+      </c>
+      <c r="I120" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" s="5">
+        <v>613232</v>
+      </c>
+      <c r="B121" s="1">
+        <v>0.251</v>
+      </c>
+      <c r="C121" s="3">
+        <f t="shared" si="12"/>
+        <v>0.749</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="19"/>
+        <v>459310.76799999998</v>
+      </c>
+      <c r="E121" s="2">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="F121" s="1">
+        <f t="shared" si="20"/>
+        <v>7.4766355140186924E-2</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="21"/>
+        <v>34340.991999999998</v>
+      </c>
+      <c r="H121">
+        <v>2008</v>
+      </c>
+      <c r="I121" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" s="5">
+        <v>573502</v>
+      </c>
+      <c r="B122" s="2">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="C122" s="3">
+        <f t="shared" si="12"/>
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="19"/>
+        <v>416935.95399999997</v>
+      </c>
+      <c r="E122" s="1">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F122" s="1">
+        <f t="shared" si="20"/>
+        <v>7.0151306740027508E-2</v>
+      </c>
+      <c r="G122">
+        <f t="shared" si="21"/>
+        <v>29248.601999999999</v>
+      </c>
+      <c r="H122">
+        <v>2007</v>
+      </c>
+      <c r="I122" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>